<commit_message>
Update: Points for Jan2
</commit_message>
<xml_diff>
--- a/pismeni-ispiti/info/202223/jan2_rezultati_vukan.xlsx
+++ b/pismeni-ispiti/info/202223/jan2_rezultati_vukan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
   <si>
     <t>Бр.</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>maks:</t>
+  </si>
+  <si>
+    <t>Skalirano:</t>
   </si>
 </sst>
 </file>
@@ -1137,19 +1140,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="27.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>103</v>
       </c>
@@ -1178,8 +1182,12 @@
         <f>SUM(D1:J1)</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1">
+        <f>ROUND((K1*65)/60, 1)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1213,8 +1221,11 @@
       <c r="K2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1228,8 +1239,12 @@
         <f>SUM(D3:J3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <f t="shared" ref="L2:L52" si="0">ROUND((K3*65)/60, 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1240,11 +1255,15 @@
         <v>6</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K52" si="0">SUM(D4:J4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" ref="K4:K52" si="1">SUM(D4:J4)</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1255,11 +1274,15 @@
         <v>8</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1270,11 +1293,15 @@
         <v>10</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1285,11 +1312,15 @@
         <v>12</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1300,11 +1331,15 @@
         <v>14</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1315,11 +1350,15 @@
         <v>16</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1330,11 +1369,15 @@
         <v>18</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1345,11 +1388,15 @@
         <v>20</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1360,11 +1407,15 @@
         <v>20</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1375,11 +1426,15 @@
         <v>23</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1390,11 +1445,15 @@
         <v>25</v>
       </c>
       <c r="K14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1426,11 +1485,15 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>43.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1441,11 +1504,15 @@
         <v>29</v>
       </c>
       <c r="K16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1456,11 +1523,15 @@
         <v>31</v>
       </c>
       <c r="K17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1471,11 +1542,15 @@
         <v>33</v>
       </c>
       <c r="K18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1486,11 +1561,15 @@
         <v>35</v>
       </c>
       <c r="K19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1522,11 +1601,15 @@
         <v>3</v>
       </c>
       <c r="K20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>47.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1558,11 +1641,15 @@
         <v>10</v>
       </c>
       <c r="K21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>57.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1573,11 +1660,15 @@
         <v>41</v>
       </c>
       <c r="K22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1588,11 +1679,15 @@
         <v>43</v>
       </c>
       <c r="K23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1603,11 +1698,15 @@
         <v>45</v>
       </c>
       <c r="K24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1618,11 +1717,15 @@
         <v>47</v>
       </c>
       <c r="K25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1654,11 +1757,15 @@
         <v>5</v>
       </c>
       <c r="K26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>47.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1669,11 +1776,15 @@
         <v>51</v>
       </c>
       <c r="K27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1684,11 +1795,15 @@
         <v>53</v>
       </c>
       <c r="K28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1699,11 +1814,15 @@
         <v>55</v>
       </c>
       <c r="K29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1735,11 +1854,15 @@
         <v>8</v>
       </c>
       <c r="K30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>48.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1750,11 +1873,15 @@
         <v>59</v>
       </c>
       <c r="K31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1765,7 +1892,7 @@
         <v>61</v>
       </c>
       <c r="D32">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -1777,20 +1904,24 @@
         <v>4</v>
       </c>
       <c r="H32">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I32">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K32">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>47.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1822,11 +1953,15 @@
         <v>0</v>
       </c>
       <c r="K33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1837,11 +1972,15 @@
         <v>65</v>
       </c>
       <c r="K34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1873,11 +2012,15 @@
         <v>0</v>
       </c>
       <c r="K35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1909,11 +2052,15 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <f t="shared" si="0"/>
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1924,11 +2071,15 @@
         <v>71</v>
       </c>
       <c r="K37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1939,11 +2090,15 @@
         <v>73</v>
       </c>
       <c r="K38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1954,11 +2109,15 @@
         <v>75</v>
       </c>
       <c r="K39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1969,11 +2128,15 @@
         <v>77</v>
       </c>
       <c r="K40">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -1984,11 +2147,15 @@
         <v>79</v>
       </c>
       <c r="K41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1999,11 +2166,15 @@
         <v>81</v>
       </c>
       <c r="K42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2035,11 +2206,15 @@
         <v>4</v>
       </c>
       <c r="K43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L43">
+        <f t="shared" si="0"/>
+        <v>48.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2050,11 +2225,15 @@
         <v>85</v>
       </c>
       <c r="K44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2065,11 +2244,15 @@
         <v>87</v>
       </c>
       <c r="K45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2080,11 +2263,15 @@
         <v>89</v>
       </c>
       <c r="K46">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2095,11 +2282,15 @@
         <v>91</v>
       </c>
       <c r="K47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2110,11 +2301,15 @@
         <v>93</v>
       </c>
       <c r="K48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2125,11 +2320,15 @@
         <v>95</v>
       </c>
       <c r="K49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2140,11 +2339,15 @@
         <v>97</v>
       </c>
       <c r="K50">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2155,11 +2358,15 @@
         <v>99</v>
       </c>
       <c r="K51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2191,8 +2398,12 @@
         <v>2.5</v>
       </c>
       <c r="K52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="0"/>
+        <v>43.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>